<commit_message>
new donut code and rlps data filtering by state in state_ghgrp_data_250730
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/raw/target_NAICS.xlsx
+++ b/state_fact_sheets/data/raw/target_NAICS.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanor/Documents/Industrial Decarbonization/industrial-decarb-policy-team/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanor/Documents/Industrial_Decarbonization/Industrial-decarb/state_fact_sheets/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8183B74-A266-F44F-B59B-0345AF0B9295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F09AE3-FC04-7F48-BD40-F1463CB8092B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="4300" windowWidth="34300" windowHeight="20880" xr2:uid="{E4220ED0-7915-324C-AC25-71CE49635D03}"/>
+    <workbookView xWindow="22520" yWindow="960" windowWidth="18440" windowHeight="25640" xr2:uid="{E4220ED0-7915-324C-AC25-71CE49635D03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$49</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -185,6 +188,18 @@
   </si>
   <si>
     <t>NAICS Code</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -581,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9E55DB-860D-F54C-BEE3-8C1BD7F40BC7}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,399 +607,547 @@
     <col min="2" max="2" width="60.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>311119</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>311221</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>311224</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>311225</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>311313</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>311314</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>311411</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>311421</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>311422</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>311423</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>311511</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>311513</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>311514</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>311611</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>311613</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>311615</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>311812</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>311919</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>311920</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>311942</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>311999</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>312120</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>312140</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>322110</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>322120</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>322130</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>322291</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>325110</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>325120</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>325130</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>325180</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>325193</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>325194</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>325199</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>325211</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>325212</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>325220</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>325311</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>325312</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>325314</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>325315</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>325320</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>325411</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>325412</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>325414</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>325611</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>325920</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>325998</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C49" xr:uid="{3F9E55DB-860D-F54C-BEE3-8C1BD7F40BC7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>